<commit_message>
Descripción de tus cambios
</commit_message>
<xml_diff>
--- a/assets/docs/ControlAsignaciones_Grupo.xlsx
+++ b/assets/docs/ControlAsignaciones_Grupo.xlsx
@@ -11,19 +11,22 @@
     <sheet state="visible" name="Implementacion" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Pruebas" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Postmortem" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Fase 2 Iniciacion y Estrategi" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Requerimiento y Planeacion" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="DiseñoImplementacion" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="owqzRhr+epvKSJO9FgeIKPcdHw5LqNrod8lVLxIYJWI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataChecksum="LvWNga3CUesMFNL11b0Kg017nK4Iz72bvmcI/jCiqg4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="383">
   <si>
     <t>CONTROL ASIGNACIONES</t>
   </si>
@@ -1070,6 +1073,108 @@
   </si>
   <si>
     <t>Fase Postmortem</t>
+  </si>
+  <si>
+    <t>Script Iniciacion/Estrategia*</t>
+  </si>
+  <si>
+    <t>10/23/2025</t>
+  </si>
+  <si>
+    <t>Bitacora(Individual)*</t>
+  </si>
+  <si>
+    <t>10/27/2025</t>
+  </si>
+  <si>
+    <t>Control Asignaciones*</t>
+  </si>
+  <si>
+    <t>Informe Final</t>
+  </si>
+  <si>
+    <t>10/25/2025</t>
+  </si>
+  <si>
+    <t>Acta Reunion*</t>
+  </si>
+  <si>
+    <t>Maestro de documento*</t>
+  </si>
+  <si>
+    <t>Acta de Iniciacion*</t>
+  </si>
+  <si>
+    <t>12pm</t>
+  </si>
+  <si>
+    <t>Reglas de funcionamiento del equipo y compromiso colectivo</t>
+  </si>
+  <si>
+    <t>10/24/2025</t>
+  </si>
+  <si>
+    <t>Full Correccion</t>
+  </si>
+  <si>
+    <t>10/28/2025</t>
+  </si>
+  <si>
+    <t>Plantilla detalle de caso de uso 1*</t>
+  </si>
+  <si>
+    <t>Plantilla detalle de caso de uso 2*</t>
+  </si>
+  <si>
+    <t>Plantilla detalle de caso de uso 3*</t>
+  </si>
+  <si>
+    <t>Requerimientos de atributo de calidad 1*</t>
+  </si>
+  <si>
+    <t>1pm</t>
+  </si>
+  <si>
+    <t>Requerimientos de atributo de calidad 2*</t>
+  </si>
+  <si>
+    <t>Requerimientos de atributo de calidad 3*</t>
+  </si>
+  <si>
+    <t>Escenario de calidad 1*</t>
+  </si>
+  <si>
+    <t>Escenario de calidad 2*</t>
+  </si>
+  <si>
+    <t>Escenario de calidad 3*</t>
+  </si>
+  <si>
+    <t>Bitacora Individual*</t>
+  </si>
+  <si>
+    <t>Log de defectos*</t>
+  </si>
+  <si>
+    <t>Control de Asignaciones*</t>
+  </si>
+  <si>
+    <t>Script Requerimiento/Planeacion*</t>
+  </si>
+  <si>
+    <t>Documento Final Requerimiento/Planeacion*</t>
+  </si>
+  <si>
+    <t>Especificacion detallada de tareas*</t>
+  </si>
+  <si>
+    <t>Plan de Calidad*</t>
+  </si>
+  <si>
+    <t>11:50pm</t>
+  </si>
+  <si>
+    <t>20 horas y 50 minutos</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1574,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1644,6 +1749,10 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="31" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1655,6 +1764,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1676,7 +1788,7 @@
     <xdr:ext cx="5772150" cy="3467100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1695,6 +1807,14 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1742,7 +1862,7 @@
     <xdr:ext cx="6238875" cy="3743325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1767,12 +1887,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>-190500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7162800" cy="4305300"/>
+    <xdr:ext cx="5676900" cy="3409950"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
@@ -1808,7 +1928,7 @@
     <xdr:ext cx="7162800" cy="4305300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1833,12 +1953,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7162800" cy="4305300"/>
+    <xdr:ext cx="4848225" cy="2914650"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
@@ -1897,6 +2017,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3731,6 +3855,995 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="32.25"/>
+    <col customWidth="1" min="3" max="3" width="17.38"/>
+    <col customWidth="1" min="13" max="13" width="28.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="23"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="52" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="40">
+        <v>60.0</v>
+      </c>
+      <c r="F8" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K8" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="52" t="s">
+        <v>365</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="40">
+        <v>60.0</v>
+      </c>
+      <c r="F9" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K9" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="18.0" customHeight="1">
+      <c r="A10" s="52" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F10" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I10" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="52" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F11" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>368</v>
+      </c>
+      <c r="H11" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>368</v>
+      </c>
+      <c r="J11" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K11" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L11" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F12" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="H12" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="J12" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="52" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F13" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I13" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K13" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L13" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="52" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F14" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>359</v>
+      </c>
+      <c r="J14" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K14" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L14" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="52" t="s">
+        <v>372</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F15" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I15" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="52" t="s">
+        <v>373</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E16" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F16" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K16" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L16" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="52" t="s">
+        <v>374</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F17" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>368</v>
+      </c>
+      <c r="H17" s="80">
+        <v>45968.0</v>
+      </c>
+      <c r="I17" s="52" t="s">
+        <v>368</v>
+      </c>
+      <c r="J17" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K17" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="52" t="s">
+        <v>375</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F18" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="80">
+        <v>45968.0</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K18" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="52" t="s">
+        <v>376</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F19" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="52" t="s">
+        <v>377</v>
+      </c>
+      <c r="B20" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F20" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I20" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="J20" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="52" t="s">
+        <v>378</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F21" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" s="80">
+        <v>45967.0</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K21" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L21" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M21" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="52" t="s">
+        <v>379</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E22" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F22" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K22" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L22" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M22" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="52" t="s">
+        <v>380</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F23" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="G23" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="I23" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K23" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L23" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F24" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G24" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="H24" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I24" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="J24" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K24" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M24" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="52">
+        <v>180.0</v>
+      </c>
+      <c r="F25" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H25" s="81">
+        <v>45968.0</v>
+      </c>
+      <c r="I25" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J25" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L25" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M25" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="52" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="52">
+        <v>50.0</v>
+      </c>
+      <c r="F26" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>381</v>
+      </c>
+      <c r="H26" s="81">
+        <v>45967.0</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>381</v>
+      </c>
+      <c r="J26" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L26" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M26" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="58">
+        <v>1250.0</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>382</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:K2"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:L6"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -9189,7 +10302,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="78"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9206,7 +10319,7 @@
       <c r="M1" s="6"/>
     </row>
     <row r="2">
-      <c r="A2" s="7"/>
+      <c r="A2" s="79"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -9351,13 +10464,13 @@
       <c r="E8" s="40">
         <v>60.0</v>
       </c>
-      <c r="F8" s="78">
+      <c r="F8" s="80">
         <v>45932.0</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="78">
+      <c r="H8" s="80">
         <v>45932.0</v>
       </c>
       <c r="I8" s="40" t="s">
@@ -9392,13 +10505,13 @@
       <c r="E9" s="40">
         <v>60.0</v>
       </c>
-      <c r="F9" s="78">
+      <c r="F9" s="80">
         <v>45932.0</v>
       </c>
       <c r="G9" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="80">
         <v>45932.0</v>
       </c>
       <c r="I9" s="40" t="s">
@@ -9433,13 +10546,13 @@
       <c r="E10" s="66">
         <v>60.0</v>
       </c>
-      <c r="F10" s="79">
+      <c r="F10" s="81">
         <v>45932.0</v>
       </c>
       <c r="G10" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="81">
         <v>45932.0</v>
       </c>
       <c r="I10" s="55" t="s">
@@ -10171,7 +11284,7 @@
       <c r="A31" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="80">
+      <c r="B31" s="82">
         <v>900.0</v>
       </c>
       <c r="C31" s="77" t="s">
@@ -10188,12 +11301,10 @@
     </row>
     <row r="38">
       <c r="A38" s="77"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="77"/>
+      <c r="B38" s="82"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="7">
     <mergeCell ref="B1:K2"/>
     <mergeCell ref="L1:M2"/>
     <mergeCell ref="A3:A4"/>
@@ -10383,13 +11494,13 @@
       <c r="E8" s="40">
         <v>60.0</v>
       </c>
-      <c r="F8" s="78">
+      <c r="F8" s="80">
         <v>45936.0</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="78">
+      <c r="H8" s="80">
         <v>45936.0</v>
       </c>
       <c r="I8" s="40" t="s">
@@ -10424,13 +11535,13 @@
       <c r="E9" s="40">
         <v>60.0</v>
       </c>
-      <c r="F9" s="78">
+      <c r="F9" s="80">
         <v>45936.0</v>
       </c>
       <c r="G9" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="80">
         <v>45936.0</v>
       </c>
       <c r="I9" s="40" t="s">
@@ -10465,13 +11576,13 @@
       <c r="E10" s="66">
         <v>60.0</v>
       </c>
-      <c r="F10" s="79">
+      <c r="F10" s="81">
         <v>45936.0</v>
       </c>
       <c r="G10" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="81">
         <v>45936.0</v>
       </c>
       <c r="I10" s="55" t="s">
@@ -10817,7 +11928,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="83" t="s">
         <v>331</v>
       </c>
       <c r="B19" s="52" t="s">
@@ -11917,6 +13028,3282 @@
       </c>
       <c r="F55" s="58" t="s">
         <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:K2"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:L6"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="41.75"/>
+    <col customWidth="1" min="13" max="13" width="26.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="23"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="52" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="40">
+        <v>60.0</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K8" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="52" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="40">
+        <v>60.0</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K9" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="I10" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K10" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L10" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="52" t="s">
+        <v>353</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K11" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L11" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="52" t="s">
+        <v>354</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>355</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="52" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I13" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K13" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L13" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="52" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="66">
+        <v>60.0</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="I14" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K14" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L14" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="66">
+        <v>270.0</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>359</v>
+      </c>
+      <c r="H15" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I15" s="55" t="s">
+        <v>359</v>
+      </c>
+      <c r="J15" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L15" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E16" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H16" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J16" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K16" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L16" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I17" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J17" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K17" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="52">
+        <v>15.0</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J18" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K18" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F19" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J19" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="52">
+        <v>20.0</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H20" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I20" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J20" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M20" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="52">
+        <v>15.0</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H21" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J21" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K21" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L21" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M21" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E22" s="52">
+        <v>15.0</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H22" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J22" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K22" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L22" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M22" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F23" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G23" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H23" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I23" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J23" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K23" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L23" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M23" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G24" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H24" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I24" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J24" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K24" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M24" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F25" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H25" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I25" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J25" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L25" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M25" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F26" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J26" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L26" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M26" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E27" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F27" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H27" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I27" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J27" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K27" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L27" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M27" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E28" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H28" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I28" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J28" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K28" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L28" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M28" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F29" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H29" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J29" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K29" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L29" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M29" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E30" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F30" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G30" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H30" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I30" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J30" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K30" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L30" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M30" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E31" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F31" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G31" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H31" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I31" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J31" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K31" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M31" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E32" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F32" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G32" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H32" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I32" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J32" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K32" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L32" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M32" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E33" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F33" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H33" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I33" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J33" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K33" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L33" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M33" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E34" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F34" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G34" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H34" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I34" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J34" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K34" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L34" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M34" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E35" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F35" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H35" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I35" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J35" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K35" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L35" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M35" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E36" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F36" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G36" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H36" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I36" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J36" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K36" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L36" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M36" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E37" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F37" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G37" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H37" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I37" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J37" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K37" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L37" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M37" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E38" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G38" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I38" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J38" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K38" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L38" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M38" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E39" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F39" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G39" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H39" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I39" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J39" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K39" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L39" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M39" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E40" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="F40" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="G40" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H40" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I40" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="J40" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K40" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L40" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M40" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="52"/>
+      <c r="B41" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K41" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L41" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M41" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="52"/>
+      <c r="B42" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K42" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L42" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M42" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="52"/>
+      <c r="B43" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K43" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L43" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M43" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="52"/>
+      <c r="B44" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K44" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L44" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M44" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I45" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K45" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L45" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M45" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G46" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I46" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J46" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K46" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L46" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M46" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I47" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J47" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K47" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L47" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M47" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G48" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I48" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J48" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K48" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L48" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M48" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I49" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J49" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K49" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L49" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M49" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G50" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H50" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I50" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J50" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K50" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L50" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M50" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G51" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I51" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J51" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K51" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L51" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M51" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G52" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I52" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J52" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K52" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L52" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M52" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G53" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H53" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I53" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J53" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K53" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L53" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M53" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G54" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I54" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K54" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L54" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M54" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G55" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H55" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I55" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J55" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K55" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L55" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M55" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G56" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I56" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J56" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K56" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L56" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M56" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G57" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H57" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I57" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J57" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K57" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L57" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M57" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G58" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H58" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I58" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J58" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K58" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L58" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M58" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G59" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I59" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J59" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K59" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L59" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M59" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G60" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H60" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I60" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J60" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K60" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L60" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M60" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E61" s="52"/>
+      <c r="F61" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G61" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H61" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I61" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J61" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K61" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L61" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M61" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G62" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H62" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I62" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J62" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K62" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L62" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M62" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G63" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H63" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I63" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J63" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K63" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L63" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M63" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E64" s="52"/>
+      <c r="F64" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G64" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H64" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I64" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J64" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K64" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L64" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M64" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G65" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H65" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I65" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J65" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K65" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L65" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M65" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E66" s="52"/>
+      <c r="F66" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G66" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H66" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I66" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J66" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K66" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L66" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M66" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E67" s="52"/>
+      <c r="F67" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G67" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H67" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I67" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J67" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K67" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L67" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M67" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E68" s="52"/>
+      <c r="F68" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H68" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I68" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J68" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K68" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L68" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M68" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="B69" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E69" s="52"/>
+      <c r="F69" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G69" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H69" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I69" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J69" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K69" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L69" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M69" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G70" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H70" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I70" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J70" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K70" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L70" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M70" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E71" s="52"/>
+      <c r="F71" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G71" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H71" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I71" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J71" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K71" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L71" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M71" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D72" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G72" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H72" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I72" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J72" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K72" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L72" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M72" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H73" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I73" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J73" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K73" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L73" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M73" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E74" s="52"/>
+      <c r="F74" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G74" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H74" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I74" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J74" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K74" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L74" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M74" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E75" s="52"/>
+      <c r="F75" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G75" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H75" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I75" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J75" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K75" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L75" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M75" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B76" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E76" s="52"/>
+      <c r="F76" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G76" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H76" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I76" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J76" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K76" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L76" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M76" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="B77" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D77" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E77" s="52"/>
+      <c r="F77" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G77" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H77" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I77" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J77" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K77" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L77" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M77" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="B78" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D78" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E78" s="52"/>
+      <c r="F78" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G78" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H78" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I78" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J78" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K78" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L78" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M78" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="B79" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E79" s="52"/>
+      <c r="F79" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G79" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H79" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I79" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J79" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K79" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L79" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M79" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B80" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D80" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E80" s="52"/>
+      <c r="F80" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="G80" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="H80" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="I80" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="J80" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K80" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L80" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M80" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="52"/>
+      <c r="B81" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E81" s="52"/>
+      <c r="F81" s="52"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="52"/>
+      <c r="I81" s="52"/>
+      <c r="J81" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K81" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L81" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M81" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="52"/>
+      <c r="B82" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D82" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E82" s="52"/>
+      <c r="F82" s="52"/>
+      <c r="G82" s="52"/>
+      <c r="H82" s="52"/>
+      <c r="I82" s="52"/>
+      <c r="J82" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K82" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L82" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M82" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="52"/>
+      <c r="B83" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E83" s="52"/>
+      <c r="F83" s="52"/>
+      <c r="G83" s="52"/>
+      <c r="H83" s="52"/>
+      <c r="I83" s="52"/>
+      <c r="J83" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K83" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L83" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M83" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="52"/>
+      <c r="B84" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D84" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E84" s="52"/>
+      <c r="F84" s="52"/>
+      <c r="G84" s="52"/>
+      <c r="H84" s="52"/>
+      <c r="I84" s="52"/>
+      <c r="J84" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K84" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L84" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M84" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="52"/>
+      <c r="B85" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D85" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E85" s="52"/>
+      <c r="F85" s="52"/>
+      <c r="G85" s="52"/>
+      <c r="H85" s="52"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K85" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L85" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M85" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D86" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E86" s="52">
+        <v>60.0</v>
+      </c>
+      <c r="F86" s="52" t="s">
+        <v>352</v>
+      </c>
+      <c r="G86" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="H86" s="52" t="s">
+        <v>352</v>
+      </c>
+      <c r="I86" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="J86" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K86" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L86" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M86" s="76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="B87" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D87" s="66">
+        <v>1.0</v>
+      </c>
+      <c r="E87" s="52">
+        <v>180.0</v>
+      </c>
+      <c r="F87" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="G87" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H87" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="I87" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="J87" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="K87" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="L87" s="45">
+        <v>0.0</v>
+      </c>
+      <c r="M87" s="76" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>